<commit_message>
update rocm summary graph
</commit_message>
<xml_diff>
--- a/tvm-amd-MI50-sycl-test-result/rocm-MI50-network-summary-new.xlsx
+++ b/tvm-amd-MI50-sycl-test-result/rocm-MI50-network-summary-new.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\王紫阳\计算所\组会PPT模板\2023\tvm-sycl-test-result-amd-MI50\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wzy\Desktop\tvm-sycl-summary\tvm-amd-MI50-sycl-test-result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF2DAE8-8237-4A7B-BBAF-984D9BBDE801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DAC54F-6FD1-4021-8045-7F8F0BEDE783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8270" yWindow="-21710" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{DC91560C-149E-49D9-93D5-99C61F8637CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DC91560C-149E-49D9-93D5-99C61F8637CA}"/>
   </bookViews>
   <sheets>
     <sheet name="MI50_alexnet" sheetId="2" r:id="rId1"/>
@@ -468,16 +468,16 @@
       <numFmt numFmtId="176" formatCode="mm:ss.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <numFmt numFmtId="176" formatCode="mm:ss.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="mm:ss.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="mm:ss.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="mm:ss.000"/>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="176" formatCode="mm:ss.000"/>
@@ -1239,6 +1239,628 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>network infer time</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MI50_shufflenet!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rocm_infer_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>MI50_shufflenet!$B$2:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>shufflenet-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>shufflenet-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>shufflenet-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shufflenet-8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>shufflenet-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>shufflenet-v2-10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MI50_shufflenet!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9.7513537115384592E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7529236153846097E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7500211153846092E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7576728141025599E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7518333910256404E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6964214876543198E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-0E5D-4990-BFF4-33685839103C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MI50_shufflenet!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rocm-libs_infer_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>MI50_shufflenet!$B$2:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>shufflenet-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>shufflenet-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>shufflenet-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shufflenet-8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>shufflenet-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>shufflenet-v2-10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MI50_shufflenet!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.7799749552845497E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7846806794871805E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7829343269230703E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7867230064102497E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7902200064102496E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3270342761237501E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-0E5D-4990-BFF4-33685839103C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MI50_shufflenet!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>opencl_infer_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>MI50_shufflenet!$B$2:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>shufflenet-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>shufflenet-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>shufflenet-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shufflenet-8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>shufflenet-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>shufflenet-v2-10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MI50_shufflenet!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.0087601515151505E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0297340530303E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0152546590909002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.9942502689393904E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.03196136904761E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3534932520325202E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-0E5D-4990-BFF4-33685839103C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MI50_shufflenet!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sycl_infer_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>MI50_shufflenet!$B$2:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>shufflenet-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>shufflenet-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>shufflenet-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shufflenet-8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>shufflenet-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>shufflenet-v2-10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MI50_shufflenet!$F$2:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.42220798703703E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.42327928518518E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.48268537962962E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.42706749537037E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.41922920648148E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3967681185185101E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-0E5D-4990-BFF4-33685839103C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="961495135"/>
+        <c:axId val="961497535"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="961495135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="961497535"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="961497535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="961495135"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.9444444444444448E-2"/>
+          <c:y val="0.82951864026705402"/>
+          <c:w val="0.9"/>
+          <c:h val="7.8017189598872966E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
               <a:t>network cost time</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN" altLang="en-US"/>
@@ -1816,7 +2438,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -2427,7 +3049,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -3039,7 +3661,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -3603,7 +4225,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -4167,7 +4789,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -4775,7 +5397,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -5363,7 +5985,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -5950,7 +6572,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -7881,6 +8503,588 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>network infer time</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MI50_efficientnet_lite4!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rocm_infer_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>MI50_efficientnet_lite4!$A$2:$B$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>efficientnet-lite4-11</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>efficientnet-lite4-11-qdq</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>efficientnet_lite4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>efficientnet_lite4</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MI50_efficientnet_lite4!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5.4107858581560198E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7626406037037002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1172-4FDE-971A-6058DD7705E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MI50_efficientnet_lite4!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rocm-libs_infer_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>MI50_efficientnet_lite4!$A$2:$B$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>efficientnet-lite4-11</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>efficientnet-lite4-11-qdq</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>efficientnet_lite4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>efficientnet_lite4</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MI50_efficientnet_lite4!$D$2:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.3809968530571898E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7393179609810402E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1172-4FDE-971A-6058DD7705E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MI50_efficientnet_lite4!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>opencl_infer_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>MI50_efficientnet_lite4!$A$2:$B$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>efficientnet-lite4-11</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>efficientnet-lite4-11-qdq</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>efficientnet_lite4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>efficientnet_lite4</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MI50_efficientnet_lite4!$E$2:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.3219088991227999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.34441483771929E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1172-4FDE-971A-6058DD7705E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MI50_efficientnet_lite4!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sycl_infer_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>MI50_efficientnet_lite4!$A$2:$B$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>efficientnet-lite4-11</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>efficientnet-lite4-11-qdq</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>efficientnet_lite4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>efficientnet_lite4</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MI50_efficientnet_lite4!$F$2:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.102554851933333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.104126747066666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1172-4FDE-971A-6058DD7705E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="84947952"/>
+        <c:axId val="84942192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="84947952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84942192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84942192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84947952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>network infer time</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8432,7 +9636,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -8988,7 +10192,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -9652,7 +10856,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -10496,7 +11700,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -11087,628 +12291,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>network infer time</a:t>
-            </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>MI50_shufflenet!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>rocm_infer_time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>MI50_shufflenet!$B$2:$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>shufflenet-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>shufflenet-6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>shufflenet-7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>shufflenet-8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>shufflenet-9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>shufflenet-v2-10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MI50_shufflenet!$C$2:$C$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>9.7513537115384592E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.7529236153846097E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.7500211153846092E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.7576728141025599E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.7518333910256404E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.6964214876543198E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-0E5D-4990-BFF4-33685839103C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>MI50_shufflenet!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>rocm-libs_infer_time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>MI50_shufflenet!$B$2:$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>shufflenet-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>shufflenet-6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>shufflenet-7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>shufflenet-8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>shufflenet-9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>shufflenet-v2-10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MI50_shufflenet!$D$2:$D$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.7799749552845497E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.7846806794871805E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.7829343269230703E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.7867230064102497E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.7902200064102496E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.3270342761237501E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-0E5D-4990-BFF4-33685839103C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>MI50_shufflenet!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>opencl_infer_time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>MI50_shufflenet!$B$2:$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>shufflenet-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>shufflenet-6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>shufflenet-7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>shufflenet-8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>shufflenet-9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>shufflenet-v2-10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MI50_shufflenet!$E$2:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.0087601515151505E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.0297340530303E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.0152546590909002E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.9942502689393904E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.03196136904761E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3534932520325202E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-0E5D-4990-BFF4-33685839103C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>MI50_shufflenet!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>sycl_infer_time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>MI50_shufflenet!$B$2:$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>shufflenet-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>shufflenet-6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>shufflenet-7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>shufflenet-8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>shufflenet-9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>shufflenet-v2-10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>MI50_shufflenet!$F$2:$F$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.42220798703703E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.42327928518518E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.48268537962962E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.42706749537037E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.41922920648148E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.3967681185185101E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-0E5D-4990-BFF4-33685839103C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="961495135"/>
-        <c:axId val="961497535"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="961495135"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="961497535"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="961497535"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="961495135"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="6.9444444444444448E-2"/>
-          <c:y val="0.82951864026705402"/>
-          <c:w val="0.9"/>
-          <c:h val="7.8017189598872966E-2"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12182,6 +12764,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -17532,6 +18154,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -21598,6 +22723,83 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>643890</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>145415</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>262890</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC3E92E7-69CD-9AD9-08C8-ACBD436E2ADE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>407670</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>13335</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>102870</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>93345</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBC77787-E943-A21A-3069-A3575A23ACE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -21674,7 +22876,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -21751,7 +22953,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -21828,7 +23030,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -21991,16 +23193,57 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>996950</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>127635</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1051560</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{363BD6EC-8C87-CFE1-5022-560540F0E6A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>59690</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>173355</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>128270</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>29845</xdr:rowOff>
+      <xdr:colOff>600710</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>75565</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22028,7 +23271,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -22069,7 +23312,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -22110,7 +23353,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -22151,7 +23394,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -22192,85 +23435,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>643890</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>145415</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>262890</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="图表 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC3E92E7-69CD-9AD9-08C8-ACBD436E2ADE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>407670</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>13335</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>102870</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>93345</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="图表 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBC77787-E943-A21A-3069-A3575A23ACE8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{924D029E-38B7-438A-B3AE-3A59500763B7}" name="表8" displayName="表8" ref="A1:J6" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{924D029E-38B7-438A-B3AE-3A59500763B7}" name="表8" displayName="表8" ref="A1:J6" totalsRowShown="0" headerRowDxfId="39">
   <autoFilter ref="A1:J6" xr:uid="{924D029E-38B7-438A-B3AE-3A59500763B7}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{977139C3-C3B8-41AE-8E92-8D0235EBAFC3}" name="network_name"/>
@@ -22279,17 +23445,17 @@
     <tableColumn id="4" xr3:uid="{599696CD-1B8E-4FA4-BE9A-E1B5813EA845}" name="rocm-libs_infer_time"/>
     <tableColumn id="5" xr3:uid="{8B4A2EC7-044B-4B93-8ED2-58EB8FF6ADD4}" name="opencl_infer_time"/>
     <tableColumn id="6" xr3:uid="{BBF2FEF5-52C8-4F16-87E3-A7D86C85AC99}" name="sycl_infer_time"/>
-    <tableColumn id="7" xr3:uid="{11867066-04D7-4797-8645-3AB1489A385E}" name="rocm_cost_time" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{31CF6E40-C26B-4CAE-8223-F08C1DBB706B}" name="rocm-libs_cost_time" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{28F349AC-DC3B-42B4-AD90-947868E87756}" name="opencl_cost_time" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{F80E1ED7-1EF1-4CFF-93C8-977E67B583AF}" name="sycl_cost_time" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{11867066-04D7-4797-8645-3AB1489A385E}" name="rocm_cost_time" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{31CF6E40-C26B-4CAE-8223-F08C1DBB706B}" name="rocm-libs_cost_time" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{28F349AC-DC3B-42B4-AD90-947868E87756}" name="opencl_cost_time" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{F80E1ED7-1EF1-4CFF-93C8-977E67B583AF}" name="sycl_cost_time" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0BA29E6E-2661-486C-A6E1-84989B778345}" name="表9" displayName="表9" ref="A1:J6" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0BA29E6E-2661-486C-A6E1-84989B778345}" name="表9" displayName="表9" ref="A1:J6" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A1:J6" xr:uid="{0BA29E6E-2661-486C-A6E1-84989B778345}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{1C913B75-8A45-4AE0-BE7C-2BC59AE7EC51}" name="network_name"/>
@@ -22298,17 +23464,17 @@
     <tableColumn id="4" xr3:uid="{6B32E9C8-A71F-4743-AA74-D0723DF9A98B}" name="rocm-libs_infer_time"/>
     <tableColumn id="5" xr3:uid="{0F997B42-F930-48FD-B0C6-BAC98AD9F0CB}" name="opencl_infer_time"/>
     <tableColumn id="6" xr3:uid="{9D87C38F-3209-45E6-A818-7533369194CC}" name="sycl_infer_time"/>
-    <tableColumn id="7" xr3:uid="{CFF5FF3B-E426-4F30-919A-78206DCC5FBF}" name="rocm_cost_time" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{AB67D769-B03F-432F-932C-A1D5A8AB81F3}" name="rocm-libs_cost_time" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{C036DC0A-CA80-4B8A-A5A7-DFEEACF98DD5}" name="opencl_cost_time" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{9664AD78-8AD8-4BCD-94BA-8F4E8A9DBB68}" name="sycl_cost_time" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{CFF5FF3B-E426-4F30-919A-78206DCC5FBF}" name="rocm_cost_time" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{AB67D769-B03F-432F-932C-A1D5A8AB81F3}" name="rocm-libs_cost_time" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{C036DC0A-CA80-4B8A-A5A7-DFEEACF98DD5}" name="opencl_cost_time" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{9664AD78-8AD8-4BCD-94BA-8F4E8A9DBB68}" name="sycl_cost_time" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{244B3EDD-6067-48A6-B65D-DF4CA2207946}" name="表5" displayName="表5" ref="A1:J6" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{244B3EDD-6067-48A6-B65D-DF4CA2207946}" name="表5" displayName="表5" ref="A1:J6" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A1:J6" xr:uid="{244B3EDD-6067-48A6-B65D-DF4CA2207946}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A981C57A-E096-45FA-BFCD-B81172024D66}" name="network_name"/>
@@ -22317,36 +23483,51 @@
     <tableColumn id="4" xr3:uid="{8C5CBC8A-EC90-4E5D-AD6C-3386D9141B36}" name="rocm-libs_infer_time"/>
     <tableColumn id="5" xr3:uid="{573281D8-2581-471A-81E2-6EC3314F1BDE}" name="opencl_infer_time"/>
     <tableColumn id="6" xr3:uid="{13F99A93-164B-4F00-8B15-974760BE5B3C}" name="sycl_infer_time"/>
-    <tableColumn id="7" xr3:uid="{A2ED8D8A-9A64-42DE-B832-42DB16F4B1B8}" name="rocm_cost_time" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{F0459770-0C67-4195-AB7F-5BA433C8E090}" name="rocm-libs_cost_time" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{E31B6C90-DF05-4974-A456-92174209126F}" name="opencl_cost_time" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{FE5D1BD8-A713-4302-B15F-C1F079B62F32}" name="sycl_cost_time" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{A2ED8D8A-9A64-42DE-B832-42DB16F4B1B8}" name="rocm_cost_time" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{F0459770-0C67-4195-AB7F-5BA433C8E090}" name="rocm-libs_cost_time" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{E31B6C90-DF05-4974-A456-92174209126F}" name="opencl_cost_time" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{FE5D1BD8-A713-4302-B15F-C1F079B62F32}" name="sycl_cost_time" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C159462B-1FB7-4B53-B148-8E091AF187E9}" name="表6" displayName="表6" ref="A1:J4" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:J4" xr:uid="{C159462B-1FB7-4B53-B148-8E091AF187E9}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{9C511885-815C-4CA5-96A2-7571F4F31B65}" name="network_name"/>
-    <tableColumn id="2" xr3:uid="{FD1ECF51-ACF0-45EE-9AA8-932D15C25558}" name="network_sub_name"/>
-    <tableColumn id="3" xr3:uid="{24065523-42B8-4D1D-B151-7E14F559CC37}" name="rocm_infer_time"/>
-    <tableColumn id="4" xr3:uid="{A1DD907F-95F2-43FA-B5B8-B96BC63A60B0}" name="rocm-libs_infer_time" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{DB3B6882-0377-4C6C-BAA4-E358F649A5F5}" name="opencl_infer_time" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{E816D285-774D-464C-9975-639D78DD7D2A}" name="sycl_infer_time"/>
-    <tableColumn id="7" xr3:uid="{15E4AFEF-188A-41BC-B6D3-EBF7F67FCF36}" name="rocm_cost_time" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{F37D2B4E-7224-4864-948A-2E90C9A5ECA3}" name="rocm-libs_cost_time" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{B900A419-6B40-41F5-B4BB-9537F2C71E1E}" name="opencl_cost_time" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{629BB172-97C8-4177-9D3F-F3108D0E6286}" name="sycl_cost_time" dataDxfId="16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{07B39C7F-0325-486A-BAD1-8454A70E3663}" name="表4" displayName="表4" ref="A1:F3" totalsRowShown="0">
+  <autoFilter ref="A1:F3" xr:uid="{07B39C7F-0325-486A-BAD1-8454A70E3663}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{374EAAFB-5BE0-41AF-A747-A14EAFC573FC}" name="network_name"/>
+    <tableColumn id="2" xr3:uid="{4368A373-88C6-4EBA-A377-58F32B320272}" name="network_sub_name"/>
+    <tableColumn id="3" xr3:uid="{6CB4E1E2-2B71-42C6-ADE3-1A67BF26C8CD}" name="rocm_infer_time"/>
+    <tableColumn id="4" xr3:uid="{43BAD7C1-4C5D-4D2B-BA19-0A03C22A4190}" name="rocm-libs_infer_time"/>
+    <tableColumn id="5" xr3:uid="{20F9F3E4-E07B-470C-9F22-4370873E0AD9}" name="opencl_infer_time"/>
+    <tableColumn id="6" xr3:uid="{B1B8EC6D-0381-4799-9735-6704DFAD4834}" name="sycl_infer_time"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{484EB5D1-073E-4267-AB16-2C7AAB042FBD}" name="表7" displayName="表7" ref="A1:J3" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C159462B-1FB7-4B53-B148-8E091AF187E9}" name="表6" displayName="表6" ref="A1:J4" totalsRowShown="0" headerRowDxfId="24">
+  <autoFilter ref="A1:J4" xr:uid="{C159462B-1FB7-4B53-B148-8E091AF187E9}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{9C511885-815C-4CA5-96A2-7571F4F31B65}" name="network_name"/>
+    <tableColumn id="2" xr3:uid="{FD1ECF51-ACF0-45EE-9AA8-932D15C25558}" name="network_sub_name"/>
+    <tableColumn id="3" xr3:uid="{24065523-42B8-4D1D-B151-7E14F559CC37}" name="rocm_infer_time"/>
+    <tableColumn id="4" xr3:uid="{A1DD907F-95F2-43FA-B5B8-B96BC63A60B0}" name="rocm-libs_infer_time" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{DB3B6882-0377-4C6C-BAA4-E358F649A5F5}" name="opencl_infer_time" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{E816D285-774D-464C-9975-639D78DD7D2A}" name="sycl_infer_time"/>
+    <tableColumn id="7" xr3:uid="{15E4AFEF-188A-41BC-B6D3-EBF7F67FCF36}" name="rocm_cost_time" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{F37D2B4E-7224-4864-948A-2E90C9A5ECA3}" name="rocm-libs_cost_time" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{B900A419-6B40-41F5-B4BB-9537F2C71E1E}" name="opencl_cost_time" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{629BB172-97C8-4177-9D3F-F3108D0E6286}" name="sycl_cost_time" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{484EB5D1-073E-4267-AB16-2C7AAB042FBD}" name="表7" displayName="表7" ref="A1:J3" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A1:J3" xr:uid="{484EB5D1-073E-4267-AB16-2C7AAB042FBD}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{3EB3C501-5C9A-4532-8F0F-6B9C3DA5F2AB}" name="network_name"/>
@@ -22355,17 +23536,17 @@
     <tableColumn id="4" xr3:uid="{211C4F5B-47DB-44AE-8C2E-ACE4701F2160}" name="rocm-libs_infer_time"/>
     <tableColumn id="5" xr3:uid="{B21B8EE9-D271-439E-8FCD-11EB3805A471}" name="opencl_infer_time"/>
     <tableColumn id="6" xr3:uid="{47540495-F1EA-47AB-8372-710B00FE0AE6}" name="sycl_infer_time"/>
-    <tableColumn id="7" xr3:uid="{17A0DE3C-3BAD-41E5-ADEA-C3144336D245}" name="rocm_cost_time" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{17DEAA1D-9232-49D6-8D99-AE680F729624}" name="rocm-libs_cost_time" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{F47B7DEC-561C-4A17-AD60-CE8FBB5E0024}" name="opencl_cost_time" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{A31EF735-8A13-458C-A7C3-4182032BA7D0}" name="sycl_cost_time" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{17A0DE3C-3BAD-41E5-ADEA-C3144336D245}" name="rocm_cost_time" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{17DEAA1D-9232-49D6-8D99-AE680F729624}" name="rocm-libs_cost_time" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{F47B7DEC-561C-4A17-AD60-CE8FBB5E0024}" name="opencl_cost_time" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{A31EF735-8A13-458C-A7C3-4182032BA7D0}" name="sycl_cost_time" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A19D8490-2766-43EC-852C-872760927483}" name="表1" displayName="表1" ref="A1:J6" totalsRowShown="0" headerRowDxfId="35">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A19D8490-2766-43EC-852C-872760927483}" name="表1" displayName="表1" ref="A1:J6" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:J6" xr:uid="{A19D8490-2766-43EC-852C-872760927483}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{48F9D5F0-F1B4-4C5A-9164-8E1E9F31CC24}" name="network_name"/>
@@ -22374,16 +23555,16 @@
     <tableColumn id="4" xr3:uid="{F1ADDC16-334B-4F8B-BAEC-E0D7E39F77C5}" name="rocm-libs_infer_time"/>
     <tableColumn id="5" xr3:uid="{99CFD146-35C5-4CFA-9F35-841FBFB2E4BB}" name="opencl_infer_time"/>
     <tableColumn id="6" xr3:uid="{125841A2-BADF-41CD-BC76-B553B504EBC6}" name="sycl_infer_time"/>
-    <tableColumn id="7" xr3:uid="{BF7DBA1D-6A55-48E2-8E2C-54583BA2D438}" name="rocm_cost_time" dataDxfId="39"/>
-    <tableColumn id="8" xr3:uid="{27C231E8-BF4C-4ABA-B176-A8F417AAA704}" name="rocm-libs_cost_time" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{DC1FCE00-36F4-47E6-8D76-66E9C4A39C0B}" name="opencl_cost_time" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{B15242FA-86C3-49CC-A5E7-74848C661BE8}" name="sycl_cost_time" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{BF7DBA1D-6A55-48E2-8E2C-54583BA2D438}" name="rocm_cost_time" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{27C231E8-BF4C-4ABA-B176-A8F417AAA704}" name="rocm-libs_cost_time" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{DC1FCE00-36F4-47E6-8D76-66E9C4A39C0B}" name="opencl_cost_time" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{B15242FA-86C3-49CC-A5E7-74848C661BE8}" name="sycl_cost_time" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2AB534D2-DD8E-4F3B-BE37-12A6AE170102}" name="表2" displayName="表2" ref="A1:M14" totalsRowShown="0">
   <autoFilter ref="A1:M14" xr:uid="{2AB534D2-DD8E-4F3B-BE37-12A6AE170102}"/>
   <tableColumns count="13">
@@ -22393,10 +23574,10 @@
     <tableColumn id="4" xr3:uid="{D7A827E6-E22A-42E0-87B7-722D69FA4E10}" name="rocm-libs_infer_time"/>
     <tableColumn id="5" xr3:uid="{D5A40D2B-F6D5-43F9-9382-BD52782542AE}" name="opencl_infer_time"/>
     <tableColumn id="6" xr3:uid="{8976BD15-7612-492E-BDF1-E42837C180EA}" name="sycl_infer_time"/>
-    <tableColumn id="7" xr3:uid="{5294D68C-8BA9-4E54-BC93-7050F5C1A7D2}" name="rocm_cost_time" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{A9DC4926-B52F-4DFD-93F3-5227927647E3}" name="rocm-libs_cost_time" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{B3367BD5-D75F-4B91-9F77-5A878FA7CD50}" name="opencl_cost_time" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{3250C8B1-2D5E-42A2-82A3-472C9C359889}" name="sycl_cost_time" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{5294D68C-8BA9-4E54-BC93-7050F5C1A7D2}" name="rocm_cost_time" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{A9DC4926-B52F-4DFD-93F3-5227927647E3}" name="rocm-libs_cost_time" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{B3367BD5-D75F-4B91-9F77-5A878FA7CD50}" name="opencl_cost_time" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{3250C8B1-2D5E-42A2-82A3-472C9C359889}" name="sycl_cost_time" dataDxfId="4"/>
     <tableColumn id="11" xr3:uid="{3CEAA763-7484-44B4-AF97-08B40E370CD0}" name="input"/>
     <tableColumn id="12" xr3:uid="{83BD7C0E-E3E9-4F67-9B4F-ED9B4DD49C5E}" name="output"/>
     <tableColumn id="13" xr3:uid="{B566E83D-E5FB-4004-9B84-F00669DDE810}" name="tolerance"/>
@@ -22405,7 +23586,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F47D98E2-72FA-4E03-AA31-C07BE971601F}" name="表3" displayName="表3" ref="A1:M12" totalsRowShown="0">
   <autoFilter ref="A1:M12" xr:uid="{F47D98E2-72FA-4E03-AA31-C07BE971601F}"/>
   <tableColumns count="13">
@@ -22415,10 +23596,10 @@
     <tableColumn id="4" xr3:uid="{DB2AA68D-5B0E-4105-8512-243732DF4AC9}" name="rocm-libs_infer_time"/>
     <tableColumn id="5" xr3:uid="{1AF3F09C-25A0-4D07-8D3D-9AF29E0D88F1}" name="opencl_infer_time"/>
     <tableColumn id="6" xr3:uid="{C48E1434-6A59-41B3-B5A9-DFB9CE47AE32}" name="sycl_infer_time"/>
-    <tableColumn id="7" xr3:uid="{4AEE7D03-593F-48FB-8062-6D2EBF4149BC}" name="rocm_cost_time" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{5D87DF2F-5819-4249-BE88-280CF04C84C9}" name="rocm-libs_cost_time" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{A74CC3AB-466C-471C-A564-6D8ECBAC616E}" name="opencl_cost_time" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{0EA92022-E5C2-45A6-B458-03F2588CA2FB}" name="sycl_cost_time" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{4AEE7D03-593F-48FB-8062-6D2EBF4149BC}" name="rocm_cost_time" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{5D87DF2F-5819-4249-BE88-280CF04C84C9}" name="rocm-libs_cost_time" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{A74CC3AB-466C-471C-A564-6D8ECBAC616E}" name="opencl_cost_time" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{0EA92022-E5C2-45A6-B458-03F2588CA2FB}" name="sycl_cost_time" dataDxfId="0"/>
     <tableColumn id="11" xr3:uid="{5BD21B0E-AB99-490F-A757-57147060C5CE}" name="input"/>
     <tableColumn id="12" xr3:uid="{3288DDCB-55BE-436E-9EA4-6105A61EBCBF}" name="output"/>
     <tableColumn id="13" xr3:uid="{6EC9495B-2616-484B-B925-2D83EF1C604B}" name="tolerance"/>
@@ -22727,7 +23908,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
@@ -25421,7 +26602,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -25810,12 +26991,17 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.77734375" customWidth="1"/>
   </cols>
@@ -26072,6 +27258,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>